<commit_message>
changes for the notes of the course 4-12-22
</commit_message>
<xml_diff>
--- a/kubernetes-manual/notes of the course.xlsx
+++ b/kubernetes-manual/notes of the course.xlsx
@@ -8,26 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\others\kubernetes-course-plural\kubernetes-manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779901A4-C8FD-43F1-92CD-0DF116A20635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27EA20D-DD2D-4B6E-A0F6-866DA2F41628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="960" windowWidth="11565" windowHeight="9075" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13170" yWindow="0" windowWidth="12660" windowHeight="8925" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="linux" sheetId="2" r:id="rId1"/>
     <sheet name="docker" sheetId="3" r:id="rId2"/>
     <sheet name="kubernetes01" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="330">
   <si>
     <t>kubernetes, course of Pluralsight , installation and configuration fundamentals by Anthony Nocetino</t>
   </si>
@@ -824,9 +833,6 @@
     <t xml:space="preserve">#we are going to append the logs on systemctl </t>
   </si>
   <si>
-    <t>Chapter 3 Docker under the hood</t>
-  </si>
-  <si>
     <t>Docker Architecture</t>
   </si>
   <si>
@@ -929,9 +935,6 @@
     <t>#it's very similar to a github respository</t>
   </si>
   <si>
-    <t>Chapter 2 Kubernetes Big Picture</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">*Store docker images called </t>
     </r>
@@ -946,13 +949,1002 @@
       </rPr>
       <t>DockerHub</t>
     </r>
+  </si>
+  <si>
+    <t>#we count the logs and we see there is an increase on the rows</t>
+  </si>
+  <si>
+    <t>cp raw_logs/master.log /tmp</t>
+  </si>
+  <si>
+    <t>egrep -v "dnf|secure" raw_logs/master.log &gt;httpd_logs/no_dnf_secure.log</t>
+  </si>
+  <si>
+    <t>#search anything different than dnf or secure and save it into the no_dnf_secure.log file</t>
+  </si>
+  <si>
+    <t>more httpd_logs/no_dnf_secure.log</t>
+  </si>
+  <si>
+    <t>###Chapter 2 Understanding and Using Essential tools on RHEL 8</t>
+  </si>
+  <si>
+    <t>################################################################</t>
+  </si>
+  <si>
+    <t>Cloud guru course</t>
+  </si>
+  <si>
+    <t>cp /etc/hosts .</t>
+  </si>
+  <si>
+    <t># we copy the hosts file to our local directory</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">####  Chapter 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Editing text files using vi/vim</t>
+    </r>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>#to delete a line in vi</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>#to delete a single character</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>#to insert and start writing characters</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>#to replace a single character</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>#to undo the previous movement</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>#redo the previous action</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>to insert a row above the current one</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>to inser a row below the current one</t>
+  </si>
+  <si>
+    <t>Docker images.</t>
+  </si>
+  <si>
+    <t>*Image is based on another image</t>
+  </si>
+  <si>
+    <t>*Read-only template with instructions for creating a docker container</t>
+  </si>
+  <si>
+    <t>*You can create  your own images</t>
+  </si>
+  <si>
+    <t>*Use Dockerfile to build images</t>
+  </si>
+  <si>
+    <t>Docker objects</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t>*Runnable instance of an image</t>
+  </si>
+  <si>
+    <t>*you can connect a container to networks</t>
+  </si>
+  <si>
+    <t>*you can attach storage</t>
+  </si>
+  <si>
+    <t>*Create a new image based on its current state</t>
+  </si>
+  <si>
+    <t>*Isolated fromother container and the host machine (you can control the level of isolation)</t>
+  </si>
+  <si>
+    <t>*Scale containers across multiple Docker daemons</t>
+  </si>
+  <si>
+    <t>* you can use docker swarm for that or kubernetes</t>
+  </si>
+  <si>
+    <t>*all the docker host are going to be able to communicate with one another using the Docker API</t>
+  </si>
+  <si>
+    <t>*there are 2 types of nodes in a docker swarm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">****And you have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>workers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that are responsible for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>executing tasks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Services allow you to define a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desired state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">**for example if you want to have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 replicas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and one of them has an issue and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dies off</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, the service will go and</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>create a new replacement replica and bring it back up to that desired state</t>
+    </r>
+  </si>
+  <si>
+    <t>*A service will go and load-balance replicas across all the worker nodes that are in the cluster</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">****you have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>managers(masters)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which are responsible for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>management of the cluster</t>
+    </r>
+  </si>
+  <si>
+    <t>########################################</t>
+  </si>
+  <si>
+    <t>###############Chapter 3 Docker under the hood</t>
+  </si>
+  <si>
+    <t>#########################################################</t>
+  </si>
+  <si>
+    <t>*Modular design</t>
+  </si>
+  <si>
+    <t>*based on the Open Container Initiative</t>
+  </si>
+  <si>
+    <t>*The Major components are</t>
+  </si>
+  <si>
+    <t>**Docker client (with this one we connect to the docker engine)</t>
+  </si>
+  <si>
+    <t>**Docker daemon (this is in the container engine area)</t>
+  </si>
+  <si>
+    <t>**containerd</t>
+  </si>
+  <si>
+    <t>**runc</t>
+  </si>
+  <si>
+    <t>these 2 work together to create and run containers</t>
+  </si>
+  <si>
+    <t>*Implementation of the OCI container runtime spec</t>
+  </si>
+  <si>
+    <t>*Lightweight CLI wrapper for libcontainer</t>
+  </si>
+  <si>
+    <t>*it creates containers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">runc   </t>
+  </si>
+  <si>
+    <t>containerd</t>
+  </si>
+  <si>
+    <t>*it manages the container lifecycle, start,stop, pause, delete</t>
+  </si>
+  <si>
+    <t>* make image management, that is push, pull images from the registry</t>
+  </si>
+  <si>
+    <t>shim</t>
+  </si>
+  <si>
+    <t>*it's used to decouple running containers from runc</t>
+  </si>
+  <si>
+    <t>how shim comes into picture, see below process…</t>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shim</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> process becomes the container parent</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>runc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> process exits after the container is created</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. when a new container is created </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>containerd forks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> an instance of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>runc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for each new container</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>above</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> steps allows to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>run hundreds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>containers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">without </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>running hundreds of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> runc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>instances</t>
+    </r>
+  </si>
+  <si>
+    <t>5. the shim is reponsible for</t>
+  </si>
+  <si>
+    <t>*STDIN and STDOUT streams open, that way if the daemond is restarted , the container doesn't go and terminate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  due to closed pipes.</t>
+  </si>
+  <si>
+    <t>6. it's also responsible to report the exit status of a container to the Docker daemon</t>
+  </si>
+  <si>
+    <t>Process Summary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">######### </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chapter 3 Docker Engine</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">######### </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chapter 3 Docker Images and Containers</t>
+    </r>
+  </si>
+  <si>
+    <t>Docker Images:</t>
+  </si>
+  <si>
+    <t>*it's a template for your containers</t>
+  </si>
+  <si>
+    <t>*An image it's like an stop container</t>
+  </si>
+  <si>
+    <t>*you can't delete an image until all the containers using that image have been deleted</t>
+  </si>
+  <si>
+    <t>*images are built from instructions in the docker file</t>
+  </si>
+  <si>
+    <t>example:</t>
+  </si>
+  <si>
+    <t>*Images are constructed of multiple layers, each one being stacked on top of the next, all layers are read-only , except the last one that is R/W</t>
+  </si>
+  <si>
+    <t>*So a container is image with a Top writable layer</t>
+  </si>
+  <si>
+    <t>*All changes are stored in the writable layer</t>
+  </si>
+  <si>
+    <t>*The writable layer is deleted when the container is deleted</t>
+  </si>
+  <si>
+    <t>In this image we have 3 container that are</t>
+  </si>
+  <si>
+    <t>using the same image, each container</t>
+  </si>
+  <si>
+    <t>has it's own R/W layer</t>
+  </si>
+  <si>
+    <t>######################################################################</t>
+  </si>
+  <si>
+    <t>########### Chapter 3 Docker hub</t>
+  </si>
+  <si>
+    <t>Docker Hub</t>
+  </si>
+  <si>
+    <t>*Public Docker registry</t>
+  </si>
+  <si>
+    <t>*Provided by Docker</t>
+  </si>
+  <si>
+    <t>*Think like github but with images</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Public and private </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repositories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, you can have unlimited public and only 1 private for free</t>
+    </r>
+  </si>
+  <si>
+    <t>*Official images… Provided by docker</t>
+  </si>
+  <si>
+    <t>*Publisher images… Provided by 3rd party vendors</t>
+  </si>
+  <si>
+    <t>this is the docker website</t>
+  </si>
+  <si>
+    <t>https://hub.docker.com</t>
+  </si>
+  <si>
+    <t>###############################</t>
+  </si>
+  <si>
+    <t>#############Chapter 2 Kubernetes Big Picture</t>
+  </si>
+  <si>
+    <t>Kubernetes Primer</t>
+  </si>
+  <si>
+    <t>Kubernetes allows you run your coud native app</t>
+  </si>
+  <si>
+    <t>but what is cloud native app?</t>
+  </si>
+  <si>
+    <t>*are built from lots of small interacting services that come together to form a useful app</t>
+  </si>
+  <si>
+    <t>Diagram of Kubernetes</t>
+  </si>
+  <si>
+    <t>##########################################</t>
+  </si>
+  <si>
+    <t>### Chapter 2 The Kubernetes API</t>
+  </si>
+  <si>
+    <t>#########################################</t>
+  </si>
+  <si>
+    <t>what is the Kubernetes API?</t>
+  </si>
+  <si>
+    <t>*Is where everything in Kubernetes is defined, example: pods deployment,etc</t>
+  </si>
+  <si>
+    <t>*it's a RESTful API, that uses standard HTTP methods or verbs to perform CRUDE(Create,Read,Update,Delete) style operations</t>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RESTful API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is an architectural style for an application program interface (API) that uses HTTP requests to access and use data. That data can be used to GET, PUT, POST,PATCH,UPDATE and DELETE data types,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*you can perform these crud operations with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kubectl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, like creating, reading and deleting objects</t>
+    </r>
+  </si>
+  <si>
+    <t>*we'll define the different parts of our apps in yaml files and we'll use kubectl to post them to the api server</t>
+  </si>
+  <si>
+    <t>Declarative Configuration</t>
+  </si>
+  <si>
+    <t>it's the Kubernetes way of deploying and managing apps</t>
+  </si>
+  <si>
+    <t>1.the kubernetes way to work is to define the various parts of those apps in yaml file,</t>
+  </si>
+  <si>
+    <t>2.you post these (yamls) to the api server as a record intent.</t>
+  </si>
+  <si>
+    <t>3.this update the overall desired state of the cluster</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. in the background the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>control plane</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is running a ton of watch loops that are constantly checking that the current observed </t>
+    </r>
+  </si>
+  <si>
+    <t>state of the cluster, matches the current desired state</t>
+  </si>
+  <si>
+    <t>5.Then control plane kick into life to bring that observed state into line with the new desired state</t>
+  </si>
+  <si>
+    <t>example let's say we change the desired state from 5 to 10 replicas</t>
+  </si>
+  <si>
+    <t>the control plane watch loops will kick off and bring the cluster to the desired state</t>
+  </si>
+  <si>
+    <t>*so the yaml files are a source of true and they server as get this living application documented</t>
+  </si>
+  <si>
+    <t>The API used to be a monlithic thing but later was decomposed to the below ones.</t>
+  </si>
+  <si>
+    <t>Also there is a group of people called the SIGs who look after them</t>
+  </si>
+  <si>
+    <t>the above SIG groups create features from Alpha, Beta and GA, you can use the below command to see the groups</t>
+  </si>
+  <si>
+    <t>################################</t>
+  </si>
+  <si>
+    <t>####### Chapter 2 Kubernetes Objects</t>
+  </si>
+  <si>
+    <t>Pods</t>
+  </si>
+  <si>
+    <t>it's the atomic unit for a k8s environment</t>
+  </si>
+  <si>
+    <t>*Contains one or more containers</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is an object on the cluster</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Atomic unit of scheduling, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>so the smallest thing you can deploy in a k8s cluster is a pod</t>
+    </r>
+  </si>
+  <si>
+    <t>*Defined in the v1 API group</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>*it's an object on the cluster</t>
+  </si>
+  <si>
+    <t>*it's a resource in the apps API group</t>
+  </si>
+  <si>
+    <t>*the pods are part of the deployment, see below</t>
+  </si>
+  <si>
+    <r>
+      <t>*it makes the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pods scalable, rolling updates and rollback simple</t>
+    </r>
+  </si>
+  <si>
+    <t>*both pods and deployments are part of the API</t>
+  </si>
+  <si>
+    <t>Deamon Sets(ds)</t>
+  </si>
+  <si>
+    <t>*They make sure that one and only one of a specific pod will run on every worker in the cluster</t>
+  </si>
+  <si>
+    <t>Stateful app components</t>
+  </si>
+  <si>
+    <t>for pods or part of your application with particular stateful requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secrets, volumes(pv) , load balancers(svc) , </t>
+  </si>
+  <si>
+    <t>Miscelaneous objects that we are not going to define here: (all are part of the API)</t>
+  </si>
+  <si>
+    <t>####### Chapter 2 Quick ways to get your own cluster</t>
+  </si>
+  <si>
+    <t>with gcp I would prefer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,12 +1959,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF858585"/>
-      <name val="Var(--chakra-fonts-heading)"/>
     </font>
     <font>
       <u/>
@@ -1022,13 +2008,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1042,31 +2050,32 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1086,6 +2095,231 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>60770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>471517</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E881A4A7-0859-4C9D-88E7-E7CA216A9126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="10919270"/>
+          <a:ext cx="6519892" cy="3149155"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>177209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C611901-FF6E-435D-971B-6BD1FB34A6DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="20202526"/>
+          <a:ext cx="3333750" cy="1891708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>218743</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>85309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4632F54-E0E4-428F-A3BA-E87C3BB8EC45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="25727025"/>
+          <a:ext cx="2657143" cy="3323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>548832</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48F1EB79-8BFB-4A9F-8D5C-E5239CAE2F43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="30870525"/>
+          <a:ext cx="4206432" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>12904</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CECB3CA7-58F2-4E52-A6B6-E2373EE462DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="34490024"/>
+          <a:ext cx="3876674" cy="3251405"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1167,6 +2401,402 @@
         <a:xfrm>
           <a:off x="17145" y="6888803"/>
           <a:ext cx="4869180" cy="2718637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85765</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1207B5B-AF7F-45CD-AF2E-E6A6D7A07DA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11430000"/>
+          <a:ext cx="9229765" cy="4619625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>398857</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>180548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEDF24F0-A58E-4737-ABDB-F39DAAA7856E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="17907000"/>
+          <a:ext cx="9542857" cy="3419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>178836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>446800</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>9113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A2E65DC-A2AA-49A3-810C-408D35F46A2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21705336"/>
+          <a:ext cx="2885200" cy="1354277"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>171968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{275D6DA0-B5A9-4661-BE81-D0105A041191}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="24260175"/>
+          <a:ext cx="6562725" cy="2200793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>26882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>372939</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1575EDC-2774-4BA2-BB5D-862E67CC147B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657975" y="24601382"/>
+          <a:ext cx="4078164" cy="1392343"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>178565</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C060922F-DDD6-4100-BB33-D1EE81DD8BB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="26679527"/>
+          <a:ext cx="5943600" cy="2074038"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>175709</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{913A89BC-26FF-4F62-B0C1-66A60D805EC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28965525"/>
+          <a:ext cx="5924550" cy="2071184"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>227482</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>130506</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B2CEB2-6C47-4DBC-8B21-1F655D793B50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="31823026"/>
+          <a:ext cx="6933082" cy="3359480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>159681</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F549E655-F3F9-4AFD-81CB-609745149966}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="35442526"/>
+          <a:ext cx="5324475" cy="2626655"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1441,384 +3071,507 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC236FEC-59ED-4862-8A34-A40E25781D78}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" ht="18.75">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+    </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+    </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+      <c r="A5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1"/>
-    </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1"/>
-    </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="1"/>
-    </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
+    <row r="30" spans="1:6">
+      <c r="A30" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
         <v>88</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
         <v>98</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>103</v>
-      </c>
-      <c r="F37" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="F38" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>108</v>
+      </c>
+      <c r="F41" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
         <v>130</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F49" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="F49" s="9" t="s">
+    <row r="50" spans="1:8">
+      <c r="F50" s="8" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F52" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F53" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F54" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
+        <v>137</v>
+      </c>
+      <c r="F55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
         <v>141</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F56" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
-      <c r="F56" t="s">
+    <row r="57" spans="1:8">
+      <c r="F57" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>144</v>
-      </c>
-      <c r="F57" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>146</v>
-      </c>
-      <c r="H58" t="s">
-        <v>148</v>
+        <v>144</v>
+      </c>
+      <c r="F58" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>147</v>
-      </c>
-      <c r="F59" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="H59" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>151</v>
-      </c>
-      <c r="H60" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="F60" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>153</v>
-      </c>
-      <c r="F61" t="s">
-        <v>152</v>
+        <v>151</v>
+      </c>
+      <c r="H61" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
         <v>154</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G63" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>174</v>
+      </c>
+      <c r="I66" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="G70" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>183</v>
+      </c>
+      <c r="G71" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>185</v>
+      </c>
+      <c r="G72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>187</v>
+      </c>
+      <c r="G73" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>189</v>
+      </c>
+      <c r="G74" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>191</v>
+      </c>
+      <c r="G75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>193</v>
+      </c>
+      <c r="G76" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>195</v>
+      </c>
+      <c r="G77" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>197</v>
+      </c>
+      <c r="G78" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1832,26 +3585,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93682837-6B4C-4833-9465-97A839E5A7F1}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1876,7 +3629,7 @@
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1911,7 +3664,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>111</v>
       </c>
       <c r="D17" t="s">
@@ -1919,75 +3672,75 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G31" t="s">
@@ -1995,26 +3748,26 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2022,135 +3775,538 @@
       <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" s="5" t="s">
         <v>112</v>
       </c>
     </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" s="4" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="4" t="s">
-        <v>165</v>
+      <c r="A47" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="4" t="s">
-        <v>167</v>
+      <c r="A53" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="3" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F57" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="15.75">
+      <c r="A75" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>229</v>
+      </c>
+      <c r="C105" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" s="12" customFormat="1">
+      <c r="A120" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
+      <c r="A179" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
+      <c r="A180" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="A181" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
+      <c r="H182" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="H183" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="H184" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1E10D46F-4B43-4C9D-A082-2D84E8D50CE8}"/>
+    <hyperlink ref="A210" r:id="rId2" xr:uid="{F5ADD71C-99C9-423E-B603-066BB9A1DD51}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A55"/>
+  <dimension ref="A1:M223"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A224" sqref="A224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -2163,20 +4319,20 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2191,7 +4347,7 @@
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2215,67 +4371,82 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:13">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="23" spans="1:13">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+    <row r="26" spans="1:13">
+      <c r="A26" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -2301,21 +4472,282 @@
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A37" r:id="rId1" xr:uid="{A5F93DB5-AD85-41F3-8979-EEF7CECF02B9}"/>
+    <hyperlink ref="A26" r:id="rId2" xr:uid="{1864EADC-3555-430B-848F-960EDA2F1B47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>